<commit_message>
update daily + request kak oyko
</commit_message>
<xml_diff>
--- a/Form Kehadiran Internship-Magang-PKL 2022.xlsx
+++ b/Form Kehadiran Internship-Magang-PKL 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muham\Desktop\Magang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90F20B2-1BD6-4AF4-BB64-BD198BF1D706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7452B411-8117-4D1B-B82F-59E7CF6B62AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Nama</t>
   </si>
@@ -166,6 +166,12 @@
     <t>- Melakukan EDA BiVi 
 - membandingkan data BiVi dan Watson
 - requesting mining data</t>
+  </si>
+  <si>
+    <t>- Mining nama nama Toko Watson pada BiVi
+- Mengenal Query data pada BiVi (mandiri), struktur database dan table.
+- mining data data hasil penjulan watson untuk beberapa lokasi
+- EDA data Watson dan BiVi</t>
   </si>
 </sst>
 </file>
@@ -748,7 +754,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -925,14 +931,22 @@
         <v>0.67708333333333337</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="4" customFormat="1" ht="43.7" customHeight="1">
+    <row r="15" spans="1:5" s="4" customFormat="1" ht="104.25" customHeight="1">
       <c r="A15" s="3">
         <v>7</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="15"/>
+      <c r="B15" s="7">
+        <v>44746</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="12">
+        <v>0.3125</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="16" spans="1:5" s="4" customFormat="1" ht="43.7" customHeight="1">
       <c r="A16" s="3">

</xml_diff>

<commit_message>
update weekly for bussines
</commit_message>
<xml_diff>
--- a/Form Kehadiran Internship-Magang-PKL 2022.xlsx
+++ b/Form Kehadiran Internship-Magang-PKL 2022.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muham\Desktop\Magang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7452B411-8117-4D1B-B82F-59E7CF6B62AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE3086B-4267-4E07-8C66-F499F76307BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Nama</t>
   </si>
@@ -172,6 +172,12 @@
 - Mengenal Query data pada BiVi (mandiri), struktur database dan table.
 - mining data data hasil penjulan watson untuk beberapa lokasi
 - EDA data Watson dan BiVi</t>
+  </si>
+  <si>
+    <t>- mining data BiVi
+- Cleaning Data BiVi
+- Exploratory Data Analysis BiVi vs Watsons
+- explore database untuk mencari data penunjang</t>
   </si>
 </sst>
 </file>
@@ -249,7 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -272,9 +278,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -287,17 +290,11 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -753,64 +750,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" style="18" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="14" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="12" customWidth="1"/>
     <col min="6" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="18" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="18" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1">
       <c r="A8" s="1" t="s">
@@ -819,7 +816,7 @@
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -836,13 +833,13 @@
       <c r="B9" s="7">
         <v>44736</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="12">
-        <v>0.3125</v>
-      </c>
-      <c r="E9" s="15">
+      <c r="D9" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E9" s="13">
         <v>0.67708333333333337</v>
       </c>
     </row>
@@ -853,13 +850,13 @@
       <c r="B10" s="7">
         <v>44739</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="12">
-        <v>0.3125</v>
-      </c>
-      <c r="E10" s="15">
+      <c r="D10" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E10" s="13">
         <v>0.70833333333333337</v>
       </c>
     </row>
@@ -870,13 +867,13 @@
       <c r="B11" s="7">
         <v>44740</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="12">
-        <v>0.3125</v>
-      </c>
-      <c r="E11" s="15">
+      <c r="D11" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E11" s="13">
         <v>0.70833333333333337</v>
       </c>
     </row>
@@ -887,13 +884,13 @@
       <c r="B12" s="7">
         <v>44741</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="12">
-        <v>0.3125</v>
-      </c>
-      <c r="E12" s="15">
+      <c r="D12" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E12" s="13">
         <v>0.70833333333333337</v>
       </c>
     </row>
@@ -904,13 +901,13 @@
       <c r="B13" s="7">
         <v>44742</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="12">
-        <v>0.3125</v>
-      </c>
-      <c r="E13" s="15">
+      <c r="D13" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E13" s="13">
         <v>0.70833333333333337</v>
       </c>
     </row>
@@ -921,13 +918,13 @@
       <c r="B14" s="7">
         <v>44743</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="12">
-        <v>0.3125</v>
-      </c>
-      <c r="E14" s="15">
+      <c r="D14" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E14" s="13">
         <v>0.67708333333333337</v>
       </c>
     </row>
@@ -938,176 +935,274 @@
       <c r="B15" s="7">
         <v>44746</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="12">
-        <v>0.3125</v>
-      </c>
-      <c r="E15" s="15">
-        <v>0.70833333333333337</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="4" customFormat="1" ht="43.7" customHeight="1">
+      <c r="D15" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="4" customFormat="1" ht="60" customHeight="1">
       <c r="A16" s="3">
         <v>8</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="15"/>
-    </row>
-    <row r="17" spans="1:5" s="4" customFormat="1" ht="43.7" customHeight="1">
+      <c r="B16" s="7">
+        <v>44747</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E16" s="13">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="4" customFormat="1" ht="61.5" customHeight="1">
       <c r="A17" s="3">
         <v>9</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="15"/>
-    </row>
-    <row r="18" spans="1:5" s="4" customFormat="1" ht="43.7" customHeight="1">
+      <c r="B17" s="7">
+        <v>44748</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E17" s="13">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="4" customFormat="1" ht="69" customHeight="1">
       <c r="A18" s="3">
         <v>10</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="15"/>
-    </row>
-    <row r="19" spans="1:5" s="4" customFormat="1" ht="43.7" customHeight="1">
+      <c r="B18" s="7">
+        <v>44749</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E18" s="13">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="4" customFormat="1" ht="66.75" customHeight="1">
       <c r="A19" s="3">
         <v>11</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="15"/>
+      <c r="B19" s="7">
+        <v>44750</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E19" s="13">
+        <v>0.67708333333333337</v>
+      </c>
     </row>
     <row r="20" spans="1:5" s="4" customFormat="1" ht="43.7" customHeight="1">
       <c r="A20" s="3">
         <v>12</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="15"/>
+      <c r="B20" s="7">
+        <v>44753</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E20" s="13">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="21" spans="1:5" s="4" customFormat="1" ht="43.7" customHeight="1">
       <c r="A21" s="3">
         <v>13</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="15"/>
+      <c r="B21" s="7">
+        <v>44754</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="22" spans="1:5" s="4" customFormat="1" ht="43.7" customHeight="1">
       <c r="A22" s="3">
         <v>14</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="15"/>
+      <c r="B22" s="7">
+        <v>44755</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E22" s="13">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="23" spans="1:5" s="4" customFormat="1" ht="43.7" customHeight="1">
       <c r="A23" s="3">
         <v>15</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="15"/>
+      <c r="B23" s="7">
+        <v>44756</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="24" spans="1:5" s="4" customFormat="1" ht="43.7" customHeight="1">
       <c r="A24" s="3">
         <v>16</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="15"/>
+      <c r="B24" s="7">
+        <v>44757</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E24" s="13">
+        <v>0.67708333333333337</v>
+      </c>
     </row>
     <row r="25" spans="1:5" s="4" customFormat="1" ht="43.7" customHeight="1">
       <c r="A25" s="3">
         <v>17</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="15"/>
+      <c r="B25" s="7">
+        <v>44760</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E25" s="13">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="26" spans="1:5" s="4" customFormat="1" ht="43.7" customHeight="1">
       <c r="A26" s="3">
         <v>18</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="15"/>
+      <c r="B26" s="7">
+        <v>44761</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E26" s="13">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="27" spans="1:5" s="4" customFormat="1" ht="43.7" customHeight="1">
       <c r="A27" s="3">
         <v>19</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="15"/>
+      <c r="B27" s="7">
+        <v>44762</v>
+      </c>
+      <c r="C27" s="17"/>
+      <c r="D27" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E27" s="13">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="28" spans="1:5" s="4" customFormat="1" ht="43.7" customHeight="1">
       <c r="A28" s="3">
         <v>20</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="15"/>
+      <c r="B28" s="7">
+        <v>44763</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E28" s="13">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="43.7" customHeight="1">
       <c r="A29" s="3">
         <v>21</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="16"/>
+      <c r="B29" s="7">
+        <v>44764</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E29" s="13">
+        <v>0.67708333333333337</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="43.7" customHeight="1">
       <c r="A30" s="3">
         <v>22</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="16"/>
+      <c r="B30" s="7">
+        <v>44767</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="11">
+        <v>0.3125</v>
+      </c>
+      <c r="E30" s="13">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="27" customHeight="1"/>
     <row r="32" spans="1:5">
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="21"/>
+      <c r="E32" s="18"/>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21" t="s">
+      <c r="C38" s="18"/>
+      <c r="D38" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="21"/>
+      <c r="E38" s="18"/>
     </row>
     <row r="39" spans="2:5" ht="19.149999999999999" customHeight="1">
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E39" s="22"/>
+      <c r="E39" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>